<commit_message>
[Documentation Update]: Enhanced project documentation and session tracking
- Updated CLAUDE.md with new auto-commit requirements (every 10 messages)
- Enhanced git_commits_log.xlsx tracking with automated updates
- Added comprehensive session summary to TRANSACTION_CARD_IMPROVEMENTS.md
- Documented mobile UI lessons learned and technical insights
- Established systematic approach for future development sessions

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Date &amp; Time</t>
   </si>
@@ -61,6 +61,9 @@
     <t>2025-08-02 08:54</t>
   </si>
   <si>
+    <t>2025-08-07 23:36</t>
+  </si>
+  <si>
     <t>81e31d9</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t>57a0da5</t>
   </si>
   <si>
+    <t>0969bf5</t>
+  </si>
+  <si>
     <t>[Documentation]: Complete transaction splitting feature documentation</t>
   </si>
   <si>
@@ -109,6 +115,9 @@
     <t>[Update]: Add gitignore for tracking files and update ping endpoint placement - Deploy: $(date '+%Y-%m-%d %H:%M')</t>
   </si>
   <si>
+    <t>[UI Enhancement]: Major mobile navigation and typography improvements</t>
+  </si>
+  <si>
     <t>Transaction splitting feature implementation</t>
   </si>
   <si>
@@ -127,7 +136,13 @@
     <t>Add gitignore for tracking files</t>
   </si>
   <si>
+    <t>Major mobile UI enhancements: Heebo font implementation, mobile navigation redesign, header/sidebar layout optimization, dashboard spacing improvements</t>
+  </si>
+  <si>
     <t>Pushed</t>
+  </si>
+  <si>
+    <t>Local</t>
   </si>
 </sst>
 </file>
@@ -485,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,10 +537,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -537,10 +552,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -548,10 +563,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -563,10 +578,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -574,10 +589,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>36</v>
@@ -589,10 +604,10 @@
         <v>195</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -600,10 +615,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -615,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -626,10 +641,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -641,10 +656,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -652,10 +667,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -667,10 +682,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -678,10 +693,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -693,10 +708,10 @@
         <v>366</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -704,10 +719,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -719,10 +734,36 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>585</v>
+      </c>
+      <c r="F10">
         <v>36</v>
       </c>
-      <c r="H9" t="s">
-        <v>37</v>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix category card weekly breakdown arrow visibility issue
Fixed CSS logic for expand arrows in category cards:
- Corrected inverted logic where arrows were hidden when collapsed and shown when expanded
- Added specific rules to hide weekly breakdown arrows when parent category is collapsed
- Weekly breakdown arrows now only show when category section is expanded

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Date &amp; Time</t>
   </si>
@@ -70,6 +70,9 @@
     <t>2025-08-08 17:01</t>
   </si>
   <si>
+    <t>2025-08-11 17:47</t>
+  </si>
+  <si>
     <t>81e31d9</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t>06a49ea</t>
   </si>
   <si>
+    <t>4becd59</t>
+  </si>
+  <si>
     <t>[Documentation]: Complete transaction splitting feature documentation</t>
   </si>
   <si>
@@ -136,6 +142,9 @@
     <t>[Critical Runtime Fixes]: Complete resolution of all Dashboard and import errors</t>
   </si>
   <si>
+    <t>[FIX]: Resolve category arrow visibility issues - eliminate duplicate arrows in shared categories</t>
+  </si>
+  <si>
     <t>Transaction splitting feature implementation</t>
   </si>
   <si>
@@ -161,6 +170,9 @@
   </si>
   <si>
     <t>Critical Runtime Fixes - Complete Dashboard and Transaction Import Resolution</t>
+  </si>
+  <si>
+    <t>Category arrow visibility fix - eliminate duplicate arrows</t>
   </si>
   <si>
     <t>Pushed</t>
@@ -524,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,10 +573,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -576,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -587,10 +599,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -602,10 +614,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -613,10 +625,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>36</v>
@@ -628,10 +640,10 @@
         <v>195</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -639,10 +651,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -654,10 +666,10 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -665,10 +677,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -680,10 +692,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -691,10 +703,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -706,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -717,10 +729,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -732,10 +744,10 @@
         <v>366</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -743,10 +755,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -758,10 +770,10 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -769,10 +781,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -784,10 +796,10 @@
         <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -795,10 +807,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -810,10 +822,10 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -821,10 +833,10 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -836,10 +848,36 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update git commits log with latest commit documentation
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Date &amp; Time</t>
   </si>
@@ -73,6 +73,9 @@
     <t>2025-08-11 17:47</t>
   </si>
   <si>
+    <t>2025-08-11 20:00</t>
+  </si>
+  <si>
     <t>81e31d9</t>
   </si>
   <si>
@@ -109,6 +112,9 @@
     <t>4becd59</t>
   </si>
   <si>
+    <t>e7098fd</t>
+  </si>
+  <si>
     <t>[Documentation]: Complete transaction splitting feature documentation</t>
   </si>
   <si>
@@ -145,6 +151,9 @@
     <t>[FIX]: Resolve category arrow visibility issues - eliminate duplicate arrows in shared categories</t>
   </si>
   <si>
+    <t>Fix category card weekly breakdown arrow visibility issue</t>
+  </si>
+  <si>
     <t>Transaction splitting feature implementation</t>
   </si>
   <si>
@@ -173,6 +182,9 @@
   </si>
   <si>
     <t>Category arrow visibility fix - eliminate duplicate arrows</t>
+  </si>
+  <si>
+    <t>Fixed category card weekly breakdown arrow visibility CSS logic</t>
   </si>
   <si>
     <t>Pushed</t>
@@ -536,7 +548,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -573,10 +585,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -588,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -599,10 +611,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -614,10 +626,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -625,10 +637,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>36</v>
@@ -640,10 +652,10 @@
         <v>195</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -651,10 +663,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -666,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -677,10 +689,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -692,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -703,10 +715,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -718,10 +730,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -729,10 +741,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -744,10 +756,10 @@
         <v>366</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -755,10 +767,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -770,10 +782,10 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -781,10 +793,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -796,10 +808,10 @@
         <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -807,10 +819,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -822,10 +834,10 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -833,10 +845,10 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -848,10 +860,10 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -859,10 +871,10 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -874,10 +886,36 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX]: Remove subscriptions page and disable RLS for custom auth
- Removed subscriptions page and route (no backend implementation)
- Removed subscriptions menu item from sidebar
- Created disable_rls_security.sql to fix cash flow data access
- Application uses custom JWT auth with service key, not Supabase Auth
- RLS conflicts with current authentication architecture

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -478,31 +478,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-08-13 23:30</t>
+          <t>2025-08-13 23:38</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fab7681</t>
+          <t>4aad170</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[SECURITY]: Pre-RLS implementation backup with current improvements</t>
+          <t>[SECURITY]: Complete RLS implementation with user context clients</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="F2" t="n">
-        <v>48</v>
+        <v>235</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pre-RLS implementation backup - UI fixes and security preparation</t>
+          <t>Complete RLS implementation - Critical security upgrade with user context clients</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>

<commit_message>
[DEBUG]: Add enhanced logging to CategoryCard monthly target loading - Deploy: 2025-08-15 08:05
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -478,31 +478,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-08-13 23:38</t>
+          <t>2025-08-15 08:03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4aad170</t>
+          <t>d825236</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[SECURITY]: Complete RLS implementation with user context clients</t>
+          <t>FIX: Resolve monthly target display issue by preventing useEffect from overriding local state updates</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>341</v>
+        <v>20</v>
       </c>
       <c r="F2" t="n">
-        <v>235</v>
+        <v>6</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Complete RLS implementation - Critical security upgrade with user context clients</t>
+          <t>Fixed monthly target display issue</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>

<commit_message>
Update git commits log with duplicate detection fix documentation
- Add detailed Hebrew documentation of Bank Scraper duplicate detection fixes
- Include technical changes and results in Excel and CSV formats
- Create summary file for quick reference

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/git_commits_log.xlsx
+++ b/git_commits_log.xlsx
@@ -1,37 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Commit Hash</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>2025-08-24</t>
+  </si>
+  <si>
+    <t>8aee52c4</t>
+  </si>
+  <si>
+    <t>Fix Bank Scraper duplicate detection system</t>
+  </si>
+  <si>
+    <t>תיקון מערכת זיהוי הכפילויות של Bank Scraper - יצירת endpoint מיוחד, תיקון סדר פרמטרים, עדכון הקליינט להשתמש ב-JSON payload במקום FormData מזויף, הוספת לוגים מפורטים, הסתרת לוגים של CategoryDropdown. כעת זיהוי כפילויות עובד תקין עבור עסקאות Bank Scraper ומציג עסקאות קיימות בצהוב.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +78,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,98 +394,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date &amp; Time</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Commit Hash</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Commit Message</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Files Changed</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Additions (+)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Deletions (-)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Session Description</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-08-16 10:28</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>7913e79</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Fix categories dropdown - use category_order table instead of category table</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>13</v>
-      </c>
-      <c r="E2" t="n">
-        <v>363</v>
-      </c>
-      <c r="F2" t="n">
-        <v>145</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Fixed categories dropdown not showing correct categories - used category_order table instead of category table</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Pushed</t>
-        </is>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>